<commit_message>
further clean up 03
</commit_message>
<xml_diff>
--- a/job_table.xlsx
+++ b/job_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bohrer/CloudMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F699A4-7DFD-8245-AB1D-57F821F4B3A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94209786-E90B-F441-BF7A-B238BF450AB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="15940" xr2:uid="{0B8EE8A8-D49C-224C-9D18-36F4097FFD55}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{0B8EE8A8-D49C-224C-9D18-36F4097FFD55}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>gseed</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>no sim</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>kernel</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Hall</t>
   </si>
 </sst>
 </file>
@@ -406,15 +421,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F85888F-B84D-8C4B-8945-9AB2A24A62F7}">
-  <dimension ref="B6:I8"/>
+  <dimension ref="B6:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -439,8 +454,14 @@
       <c r="I6" t="s">
         <v>6</v>
       </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>1</v>
       </c>
@@ -465,16 +486,22 @@
       <c r="I7" t="s">
         <v>8</v>
       </c>
+      <c r="J7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8">
-        <v>2100</v>
+        <v>2101</v>
       </c>
       <c r="D8">
-        <v>2100</v>
+        <v>2101</v>
       </c>
       <c r="E8">
         <v>75</v>
@@ -490,6 +517,76 @@
       </c>
       <c r="I8" t="s">
         <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3001</v>
+      </c>
+      <c r="D9">
+        <v>3001</v>
+      </c>
+      <c r="E9">
+        <v>75</v>
+      </c>
+      <c r="F9">
+        <v>16</v>
+      </c>
+      <c r="G9">
+        <v>24</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>3101</v>
+      </c>
+      <c r="D10">
+        <v>3101</v>
+      </c>
+      <c r="E10">
+        <v>75</v>
+      </c>
+      <c r="F10">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>24</v>
+      </c>
+      <c r="H10">
+        <v>30</v>
+      </c>
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
further clean up 04: state WITH relax-term-test
</commit_message>
<xml_diff>
--- a/job_table.xlsx
+++ b/job_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bohrer/CloudMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94209786-E90B-F441-BF7A-B238BF450AB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE68733-58D3-E441-B327-6245774B706E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{0B8EE8A8-D49C-224C-9D18-36F4097FFD55}"/>
   </bookViews>
@@ -424,7 +424,7 @@
   <dimension ref="B6:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
further clean up 05
</commit_message>
<xml_diff>
--- a/job_table.xlsx
+++ b/job_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bohrer/CloudMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE68733-58D3-E441-B327-6245774B706E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC51ADF-84CF-C843-81E9-06E99EC28189}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{0B8EE8A8-D49C-224C-9D18-36F4097FFD55}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
   <si>
     <t>gseed</t>
   </si>
@@ -70,6 +70,30 @@
   </si>
   <si>
     <t>Hall</t>
+  </si>
+  <si>
+    <t>with relax-term-tests</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>TESTS</t>
+  </si>
+  <si>
+    <t>fertige grids:</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>NaCl</t>
+  </si>
+  <si>
+    <t>errors</t>
   </si>
 </sst>
 </file>
@@ -421,15 +445,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F85888F-B84D-8C4B-8945-9AB2A24A62F7}">
-  <dimension ref="B6:K10"/>
+  <dimension ref="B6:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -460,8 +487,11 @@
       <c r="K6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>1</v>
       </c>
@@ -492,8 +522,11 @@
       <c r="K7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>2</v>
       </c>
@@ -524,8 +557,11 @@
       <c r="K8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>3</v>
       </c>
@@ -556,8 +592,11 @@
       <c r="K9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>4</v>
       </c>
@@ -587,6 +626,188 @@
       </c>
       <c r="K10" t="s">
         <v>14</v>
+      </c>
+      <c r="L10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>4001</v>
+      </c>
+      <c r="D20">
+        <v>4001</v>
+      </c>
+      <c r="E20">
+        <v>15</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="I20" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>4021</v>
+      </c>
+      <c r="D21">
+        <v>4021</v>
+      </c>
+      <c r="E21">
+        <v>15</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>5001</v>
+      </c>
+      <c r="D22">
+        <v>5001</v>
+      </c>
+      <c r="E22">
+        <v>15</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>5051</v>
+      </c>
+      <c r="D23">
+        <v>5051</v>
+      </c>
+      <c r="E23">
+        <v>15</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+      <c r="H23" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before simulation with relax with Hall on server
</commit_message>
<xml_diff>
--- a/job_table.xlsx
+++ b/job_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bohrer/CloudMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC51ADF-84CF-C843-81E9-06E99EC28189}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458D0C05-3FF3-334C-9B6E-47E9C1D677A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{0B8EE8A8-D49C-224C-9D18-36F4097FFD55}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="23">
   <si>
     <t>gseed</t>
   </si>
@@ -445,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F85888F-B84D-8C4B-8945-9AB2A24A62F7}">
-  <dimension ref="B6:M23"/>
+  <dimension ref="B2:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,6 +456,76 @@
     <col min="12" max="12" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1001</v>
+      </c>
+      <c r="D3">
+        <v>1001</v>
+      </c>
+      <c r="E3">
+        <v>75</v>
+      </c>
+      <c r="F3">
+        <v>26</v>
+      </c>
+      <c r="G3">
+        <v>38</v>
+      </c>
+      <c r="H3">
+        <v>50</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
before config file merging to one file
</commit_message>
<xml_diff>
--- a/job_table.xlsx
+++ b/job_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bohrer/CloudMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF30CDF2-10F9-2343-962D-379056EBF25D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E77484-C447-7045-B940-868B90327250}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{0B8EE8A8-D49C-224C-9D18-36F4097FFD55}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="29">
   <si>
     <t>gseed</t>
   </si>
@@ -102,25 +102,16 @@
     <t>start</t>
   </si>
   <si>
-    <t>finish</t>
-  </si>
-  <si>
-    <t>25.1.</t>
-  </si>
-  <si>
-    <t>26.1.</t>
-  </si>
-  <si>
-    <t>duration</t>
-  </si>
-  <si>
-    <t>27h</t>
-  </si>
-  <si>
-    <t>27.01., 10:50</t>
-  </si>
-  <si>
     <t>relaxation term</t>
+  </si>
+  <si>
+    <t>DNC1</t>
+  </si>
+  <si>
+    <t>DNC2</t>
+  </si>
+  <si>
+    <t>31.1.</t>
   </si>
 </sst>
 </file>
@@ -475,7 +466,7 @@
   <dimension ref="B1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,16 +512,16 @@
         <v>12</v>
       </c>
       <c r="L2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
         <v>24</v>
-      </c>
-      <c r="N2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2">
@@ -567,14 +558,11 @@
       <c r="L3" t="s">
         <v>16</v>
       </c>
-      <c r="M3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" t="s">
-        <v>29</v>
+      <c r="M3">
+        <v>60</v>
+      </c>
+      <c r="N3">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
@@ -611,8 +599,11 @@
       <c r="L4" t="s">
         <v>16</v>
       </c>
-      <c r="M4" t="s">
-        <v>30</v>
+      <c r="M4">
+        <v>60</v>
+      </c>
+      <c r="N4">
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
@@ -622,6 +613,24 @@
       <c r="C5">
         <v>3001</v>
       </c>
+      <c r="D5">
+        <v>3001</v>
+      </c>
+      <c r="E5">
+        <v>75</v>
+      </c>
+      <c r="F5">
+        <v>26</v>
+      </c>
+      <c r="G5">
+        <v>38</v>
+      </c>
+      <c r="H5">
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
       <c r="J5" t="s">
         <v>21</v>
       </c>
@@ -630,6 +639,97 @@
       </c>
       <c r="L5" t="s">
         <v>16</v>
+      </c>
+      <c r="M5">
+        <v>60</v>
+      </c>
+      <c r="N5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4001</v>
+      </c>
+      <c r="D6">
+        <v>4001</v>
+      </c>
+      <c r="E6">
+        <v>75</v>
+      </c>
+      <c r="F6">
+        <v>26</v>
+      </c>
+      <c r="G6">
+        <v>38</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="I6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6">
+        <v>30</v>
+      </c>
+      <c r="N6">
+        <v>20</v>
+      </c>
+      <c r="O6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>5001</v>
+      </c>
+      <c r="D7">
+        <v>5001</v>
+      </c>
+      <c r="E7">
+        <v>75</v>
+      </c>
+      <c r="F7">
+        <v>26</v>
+      </c>
+      <c r="G7">
+        <v>38</v>
+      </c>
+      <c r="H7">
+        <v>50</v>
+      </c>
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7">
+        <v>120</v>
+      </c>
+      <c r="N7">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
before clean-up in microphysics
</commit_message>
<xml_diff>
--- a/job_table.xlsx
+++ b/job_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bohrer/CloudMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838C4C69-5E49-F54B-A771-A383ED3152D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4111A64-FB52-EA42-A220-4D69A3F76207}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{0B8EE8A8-D49C-224C-9D18-36F4097FFD55}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="31">
   <si>
     <t>gseed</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>REPEAT NO 1 with no relax in spin up phase</t>
+  </si>
+  <si>
+    <t>17.2., 16:45</t>
   </si>
 </sst>
 </file>
@@ -466,7 +469,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F85888F-B84D-8C4B-8945-9AB2A24A62F7}">
-  <dimension ref="B1:O27"/>
+  <dimension ref="B1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
@@ -478,12 +481,12 @@
     <col min="13" max="13" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -527,7 +530,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>1</v>
       </c>
@@ -568,7 +571,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2</v>
       </c>
@@ -609,7 +612,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>3</v>
       </c>
@@ -650,7 +653,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>4</v>
       </c>
@@ -694,7 +697,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>5</v>
       </c>
@@ -735,7 +738,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>6</v>
       </c>
@@ -769,11 +772,20 @@
       <c r="L8" t="s">
         <v>16</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8">
+        <v>60</v>
+      </c>
+      <c r="N8">
+        <v>40</v>
+      </c>
+      <c r="O8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>2</v>
       </c>
@@ -808,7 +820,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>1</v>
       </c>
@@ -843,7 +855,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>2</v>
       </c>
@@ -878,7 +890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>3</v>
       </c>
@@ -913,7 +925,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>4</v>
       </c>

</xml_diff>